<commit_message>
- Corrected small bug in laser scanning, scan axis calibration for triangle waveform maximum scan frequency measurement - Scan axis calibration enters an infinite loop when testing maximum triangle waveform scan apeed at a waveform amplitude of 30 mV. This is because due to noise, the software overload detection fails and always detects an overload which does not happen. Either the overload detection should be changed, the calibration threshold should be higher or there should be some sort of lower bound for scan slope which in this case is constantly reduced. - added known issues file to keep track of known bugs.
</commit_message>
<xml_diff>
--- a/Known issues.xlsx
+++ b/Known issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Issue description</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Handle DAQmx errors when setting up DAQmx tasks and couple them to the task controller state. If an error is encountered while setting up a DAQmx task, then the task controller should be switched to an Unconfigured state so that it cannot be executed from the task tree</t>
+  </si>
+  <si>
+    <t>When a task controller is dropped as a child of another task controller in the Task Tree, the selection jumps back to the first element in the Task Tree. This is because the task tree is re-assembled each time an a task controller item is dragged and dropped. This gives a slightly annoying user experience when assembing task trees.</t>
+  </si>
+  <si>
+    <t>Laser Scanning, galvo axis calibration</t>
+  </si>
+  <si>
+    <t>When interrupting a scan axis calibration in progress by pressing the stop button on the UITC, often a General Protection Fault error is thrown. The scan calibration should be able to stop in a more reliable way.</t>
+  </si>
+  <si>
+    <t>Reported by</t>
+  </si>
+  <si>
+    <t>Adrian</t>
   </si>
 </sst>
 </file>
@@ -425,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,10 +452,12 @@
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="95.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -454,13 +471,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45">
+    <row r="2" spans="1:7" ht="45">
       <c r="A2" s="9">
         <v>42024</v>
       </c>
@@ -473,10 +493,12 @@
       <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="9">
         <v>42024</v>
       </c>
@@ -489,10 +511,12 @@
       <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="45">
+    <row r="4" spans="1:7" ht="45">
       <c r="A4" s="9">
         <v>42024</v>
       </c>
@@ -505,26 +529,48 @@
       <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="9"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
+    <row r="5" spans="1:7" ht="60">
+      <c r="A5" s="9">
+        <v>42024</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
+    <row r="6" spans="1:7" ht="45">
+      <c r="A6" s="9">
+        <v>42024</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="9"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -532,7 +578,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="9"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -540,7 +586,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -548,7 +594,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="9"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -556,7 +602,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="9"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -564,7 +610,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="9"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -572,7 +618,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="9"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -580,7 +626,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="9"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -588,7 +634,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="9"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -596,7 +642,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="9"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>

</xml_diff>

<commit_message>
- can get now scan signals from laser scanning module using galvo calibrations. - some problems occurs for images of  a few pixels. - minor memory leaks seen during scanning - only continuous scanning mode available for now, because the scan engine is sending only repeated waveform data types even for finite scans. The daqmx module can't yet cope with repeated waveforms when set to finite AO generation. - galvos are not starting or being returned to their parking position by the daqmx module when stopped.
</commit_message>
<xml_diff>
--- a/Known issues.xlsx
+++ b/Known issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Issue description</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Adrian</t>
+  </si>
+  <si>
+    <t>Develop a uniform naming system for Vchans and modify DLGetUniqueVChanName. The naming convention should be "&lt;module name&gt;: &lt;task controller name&gt;: &lt;VChanName&gt; &lt;number&gt;" with the number being optional in case there would be multiple Vchans with the same name. One issue to address in this case is how to change the VChan name if the module or task controller names change</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>DAQLab, task controller</t>
+  </si>
+  <si>
+    <t>If an error is encountered when executing an UITC and after that the UITC is reset and started again, then the UITC receives a Start event while it is stuck in its Configured state. This is seen when the UITC has child TCs, and it is possible that there is some sort of race condition again between threads. Sometimes an error does not need to occur, it seems that the reset itself is just unreliable.</t>
   </si>
 </sst>
 </file>
@@ -443,7 +455,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,20 +582,40 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="9"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
+    <row r="7" spans="1:7" ht="60">
+      <c r="A7" s="9">
+        <v>42025</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="9"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
+    <row r="8" spans="1:7" ht="60">
+      <c r="A8" s="9">
+        <v>42025</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:7">

</xml_diff>

<commit_message>
- implemented separate task controller settings for frame scan and point scan in laser scanning module. - next: implementing fluorescence recording. Just need to process incoming fluorescence signals from single point scans. Fluorescence recording is not implemented for point group jump mode.
</commit_message>
<xml_diff>
--- a/Known issues.xlsx
+++ b/Known issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Issue description</t>
   </si>
@@ -48,9 +48,6 @@
     <t>DAQmx, function AddDAQmxChannel</t>
   </si>
   <si>
-    <t>Implement a more rigorous way of generating names for VChans that must be unique. Modify DLGetUniquevChanName to make use of the module and task controller names</t>
-  </si>
-  <si>
     <t>DAQLab</t>
   </si>
   <si>
@@ -63,28 +60,22 @@
     <t>When a task controller is dropped as a child of another task controller in the Task Tree, the selection jumps back to the first element in the Task Tree. This is because the task tree is re-assembled each time an a task controller item is dragged and dropped. This gives a slightly annoying user experience when assembing task trees.</t>
   </si>
   <si>
-    <t>Laser Scanning, galvo axis calibration</t>
-  </si>
-  <si>
-    <t>When interrupting a scan axis calibration in progress by pressing the stop button on the UITC, often a General Protection Fault error is thrown. The scan calibration should be able to stop in a more reliable way.</t>
-  </si>
-  <si>
     <t>Reported by</t>
   </si>
   <si>
     <t>Adrian</t>
   </si>
   <si>
-    <t>Develop a uniform naming system for Vchans and modify DLGetUniqueVChanName. The naming convention should be "&lt;module name&gt;: &lt;task controller name&gt;: &lt;VChanName&gt; &lt;number&gt;" with the number being optional in case there would be multiple Vchans with the same name. One issue to address in this case is how to change the VChan name if the module or task controller names change</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>DAQLab, task controller</t>
-  </si>
-  <si>
-    <t>If an error is encountered when executing an UITC and after that the UITC is reset and started again, then the UITC receives a Start event while it is stuck in its Configured state. This is seen when the UITC has child TCs, and it is possible that there is some sort of race condition again between threads. Sometimes an error does not need to occur, it seems that the reset itself is just unreliable.</t>
+    <t>Laser scanning and DAQmx interaction</t>
+  </si>
+  <si>
+    <t>When AI sampling rate is 200 KHz and 3x oversampling is used, so that an actual sampling rate of 600 KHz is used for a 5us pixel dwell time, then the image looks bad. For other values of the oversampling such as 1,2,4,5 the image looks good.  Investigate why other values for the pixel dwell time such as 3.125 us give a bad image. Is the algorithm going wrong somewhere ??</t>
+  </si>
+  <si>
+    <t>data storage</t>
+  </si>
+  <si>
+    <t>If Rawdata default directory is not present, then create it by default.</t>
   </si>
 </sst>
 </file>
@@ -455,7 +446,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -483,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -506,26 +497,16 @@
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="30">
-      <c r="A3" s="9">
-        <v>42024</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
+    <row r="3" spans="1:7">
+      <c r="A3" s="9"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="45">
@@ -539,10 +520,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -551,71 +532,61 @@
         <v>42024</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:7" ht="60">
       <c r="A6" s="9">
-        <v>42024</v>
+        <v>42168</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="9">
+        <v>42168</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="60">
-      <c r="A7" s="9">
-        <v>42025</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="60">
-      <c r="A8" s="9">
-        <v>42025</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
+    <row r="8" spans="1:7">
+      <c r="A8" s="9"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:7">

</xml_diff>

<commit_message>
- changed data storage to store data only if there is at least one open VChan. The user can tick/untick the VChans for which data needs to be saved. - found a task controller error that was seen before but it seems it was not solved for all cases such as setting the task controller to execute in parallel with child TCs
</commit_message>
<xml_diff>
--- a/Known issues.xlsx
+++ b/Known issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Issue description</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>If Rawdata default directory is not present, then create it by default.</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>task controller</t>
+  </si>
+  <si>
+    <t>if task controller is set to iterate in parallel with child TCs then it receives an iteration event while it is in a done state. This error was seen before but it was corrected. It seems that it was corrected only for the case when the task controller is set to iterate before child TCs. In this case everything works fine. To reproduce the error, set up an UITC, add the scan engine as child and set it to iterate in parallel with child TCs. Add as children to the scan engine the DAQdev and pockells modules. Then set the UITC to do multiple iterations.</t>
   </si>
 </sst>
 </file>
@@ -443,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D13" sqref="D8:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -501,26 +510,36 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="9"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
+    <row r="3" spans="1:7" ht="45">
+      <c r="A3" s="9">
+        <v>42024</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="45">
+    <row r="4" spans="1:7" ht="60">
       <c r="A4" s="9">
         <v>42024</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>15</v>
@@ -529,56 +548,54 @@
     </row>
     <row r="5" spans="1:7" ht="60">
       <c r="A5" s="9">
-        <v>42024</v>
+        <v>42168</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="60">
+    <row r="6" spans="1:7">
       <c r="A6" s="9">
         <v>42168</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="90">
       <c r="A7" s="9">
-        <v>42168</v>
+        <v>42205</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:7">
@@ -766,27 +783,19 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="9"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="10"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="2"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Corrected pulse train enums in DataTypes.h because it would not include the correct value due to nidaqmx.h not defining some defines before. Now removed all DAQmx defines in DataTypes.h and daqmx specific defines are only found in the daqmx module.
- Implemented Chameleon Ti:Sa control. It's working rather well, but COM port settings are hard coded and should be made more flexible.

- Corrected daqmx counter discard and use of enum values.
</commit_message>
<xml_diff>
--- a/Known issues.xlsx
+++ b/Known issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Issue description</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>if task controller is set to iterate in parallel with child TCs then it receives an iteration event while it is in a done state. This error was seen before but it was corrected. It seems that it was corrected only for the case when the task controller is set to iterate before child TCs. In this case everything works fine. To reproduce the error, set up an UITC, add the scan engine as child and set it to iterate in parallel with child TCs. Add as children to the scan engine the DAQdev and pockells modules. Then set the UITC to do multiple iterations.</t>
+  </si>
+  <si>
+    <t>task controller and Vchans</t>
+  </si>
+  <si>
+    <t>When removing a task controller from the task tree, its source Vchans are not sending data anymore to SinkVChans belonging to the task tree, and the task tree execution will time out. To correct this, Source Vchans should be also associated (and registered) with task controllers so that they are disconnected from their sinks if the task controller is removed from the task tree</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D8:D13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -595,15 +601,27 @@
       <c r="D7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="9"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
+    <row r="8" spans="1:7" ht="60">
+      <c r="A8" s="9">
+        <v>42205</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:7">

</xml_diff>

<commit_message>
1. Pockells cell ---------------------- - Fixed bug when closing panel
2. PI Z stage
-----------------------
- Fixed bug when loading, it did not register its task controller with the framework and task tree could not be assembled
- Fixed bug when starting task controller and rel move was 0, it would jump to the target absolute position from which it would do a stack. Now if rel move is 0, it doesn't move if task controller is started.

3. Laser control
-----------------------
- timer polling laser status is now discarded before closing COM port.
</commit_message>
<xml_diff>
--- a/Known issues.xlsx
+++ b/Known issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Issue description</t>
   </si>
@@ -84,13 +84,16 @@
     <t>task controller</t>
   </si>
   <si>
-    <t>if task controller is set to iterate in parallel with child TCs then it receives an iteration event while it is in a done state. This error was seen before but it was corrected. It seems that it was corrected only for the case when the task controller is set to iterate before child TCs. In this case everything works fine. To reproduce the error, set up an UITC, add the scan engine as child and set it to iterate in parallel with child TCs. Add as children to the scan engine the DAQdev and pockells modules. Then set the UITC to do multiple iterations.</t>
-  </si>
-  <si>
     <t>task controller and Vchans</t>
   </si>
   <si>
     <t>When removing a task controller from the task tree, its source Vchans are not sending data anymore to SinkVChans belonging to the task tree, and the task tree execution will time out. To correct this, Source Vchans should be also associated (and registered) with task controllers so that they are disconnected from their sinks if the task controller is removed from the task tree</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Stopping a task controller from iterating in continuous mode often causes the error "Iterate event is invalid for Done state". This is not seen when settings the task controller to finite iterations, presumably because in Idle state iterate events are ignored. The iterate event that causes this problem is sent from the Iteration Function Active State. See file "task controller error.txt"</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,6 +166,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,9 +482,10 @@
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="48.28515625" customWidth="1"/>
+    <col min="8" max="8" width="74.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:8" ht="29.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -494,11 +504,14 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="45">
+      <c r="H1" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" s="9">
         <v>42024</v>
       </c>
@@ -515,8 +528,10 @@
         <v>15</v>
       </c>
       <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="45">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="45">
       <c r="A3" s="9">
         <v>42024</v>
       </c>
@@ -533,8 +548,10 @@
         <v>15</v>
       </c>
       <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="60">
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" ht="60">
       <c r="A4" s="9">
         <v>42024</v>
       </c>
@@ -551,8 +568,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="60">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="9">
         <v>42168</v>
       </c>
@@ -569,8 +588,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="9">
         <v>42168</v>
       </c>
@@ -587,44 +608,50 @@
         <v>15</v>
       </c>
       <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="90">
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" ht="60">
       <c r="A7" s="9">
         <v>42205</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" ht="60">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="9">
-        <v>42205</v>
+        <v>42217</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -632,7 +659,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="9"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -640,7 +667,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="9"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -648,7 +675,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="9"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -656,7 +683,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="9"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -664,7 +691,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="9"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -672,7 +699,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="9"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -680,7 +707,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="9"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -793,27 +820,19 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="9"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="10"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="6"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="2"/>
+      <c r="A32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>